<commit_message>
1.change name of notebook for M1, 2. add metadata on Covid, Stringency imported datasets 3. adding final varibales to the excel metadata file from global variables of the script
</commit_message>
<xml_diff>
--- a/Projects/M1 and M2/Suppl_info/Metadata_project_M1_M2.xlsx
+++ b/Projects/M1 and M2/Suppl_info/Metadata_project_M1_M2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubencito/CAS_datascience/ADS_CAS_Bern_2020/Projects/M1 and M2/Suppl_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E02F102-C71B-6041-92C8-CEDA28D4143A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB27569-2996-1A40-B53D-D51616D381B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="800" windowWidth="37300" windowHeight="22100" xr2:uid="{39CC3442-12D6-A64A-A909-CE0BEEB4DF0A}"/>
+    <workbookView xWindow="2320" yWindow="800" windowWidth="44500" windowHeight="25860" xr2:uid="{39CC3442-12D6-A64A-A909-CE0BEEB4DF0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,25 +25,326 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="98">
   <si>
     <t>Variable_name</t>
   </si>
   <si>
     <t>Plot_name</t>
+  </si>
+  <si>
+    <t>group?</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>urls</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>confirmed_df</t>
+  </si>
+  <si>
+    <t>deaths_df</t>
+  </si>
+  <si>
+    <t>recovered_df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of 3 urls addreses from the JH Github repository to get the raw timeseries dataset on global confirmed, death and recovery cases respectively. </t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>dataframe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data frame with time series on confirmed cases in wide format </t>
+  </si>
+  <si>
+    <t>Data frame with time series on death cases in wide format</t>
+  </si>
+  <si>
+    <t>Data frame with time series on recovered cases in wide format</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>get current working directory to store output files</t>
+  </si>
+  <si>
+    <t>dates</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>temporary character vector to construct the dates from the time series of the COVID</t>
+  </si>
+  <si>
+    <t>confirmed_df_long</t>
+  </si>
+  <si>
+    <t>deaths_df_long</t>
+  </si>
+  <si>
+    <t>recovered_df_long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data frame with time series on confirmed cases in long format </t>
+  </si>
+  <si>
+    <t>Data frame with time series on death cases in long format</t>
+  </si>
+  <si>
+    <t>Data frame with time series on recovered cases in long format</t>
+  </si>
+  <si>
+    <t>full_table</t>
+  </si>
+  <si>
+    <t>merged df containing timeseries of global cases of confirmed, deaths and recovered cases</t>
+  </si>
+  <si>
+    <t>ship_rows</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>full_grouped</t>
+  </si>
+  <si>
+    <t>sum values (cumulative sum) of grouped dataframe by Date and Country of Covid timeseries</t>
+  </si>
+  <si>
+    <t>covid_metadata_countries</t>
+  </si>
+  <si>
+    <t>raw metadata on convid dataset including Country code and country population</t>
+  </si>
+  <si>
+    <t>ship_metadata</t>
+  </si>
+  <si>
+    <t>boolean generated to filter rows containing cruise ships data on full_table dataframe</t>
+  </si>
+  <si>
+    <t>boolean generated to filter rows containing cruise ships data on covid_metadata_countries dataframe</t>
+  </si>
+  <si>
+    <t>code_vars</t>
+  </si>
+  <si>
+    <t>Variable names used for grouping covid_metadata_countries dataframe</t>
+  </si>
+  <si>
+    <t>country_population</t>
+  </si>
+  <si>
+    <t>dataframe containing information on country names, country codes and population</t>
+  </si>
+  <si>
+    <t>full_grouped_ccode</t>
+  </si>
+  <si>
+    <t>stringency</t>
+  </si>
+  <si>
+    <t>merged dataframe of Covid data that include population and country codes</t>
+  </si>
+  <si>
+    <t>my_string_columns</t>
+  </si>
+  <si>
+    <t>str_url</t>
+  </si>
+  <si>
+    <t>stringency_raw_dataset</t>
+  </si>
+  <si>
+    <t>stringe_natio_dataset</t>
+  </si>
+  <si>
+    <t>names of selected columns to import from the raw estringency index dataset</t>
+  </si>
+  <si>
+    <t>url from github repository of Stringency index from the Oxford Univeristy</t>
+  </si>
+  <si>
+    <t>raw dataframe on stringency index</t>
+  </si>
+  <si>
+    <t>filtered stringency index dataframe with only national data</t>
+  </si>
+  <si>
+    <t>full_grouped_ccode_filtered</t>
+  </si>
+  <si>
+    <t>filtered datarame of covid timeseries cases with only countries included in the stringency index dataset</t>
+  </si>
+  <si>
+    <t>my_complete_df</t>
+  </si>
+  <si>
+    <t>Joined dataframe with covid cases and stringency index</t>
+  </si>
+  <si>
+    <t>my_countries_dicc</t>
+  </si>
+  <si>
+    <t>dictionary</t>
+  </si>
+  <si>
+    <t>pair of values to identify contry names by standarized country codes</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>assigned country character value to be ploted/analyzed</t>
+  </si>
+  <si>
+    <t>single_country_covid_df</t>
+  </si>
+  <si>
+    <t>dotaframe of covid cases and stringency index timeseries of specified country</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>counter to initialize the loop for ploting covid dataframe</t>
+  </si>
+  <si>
+    <t>my_home_url</t>
+  </si>
+  <si>
+    <t>my_params</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>socioeconomics</t>
+  </si>
+  <si>
+    <t>my_vars_for_ploting</t>
+  </si>
+  <si>
+    <t>list of names with variables in the joined covidd df for ploting</t>
+  </si>
+  <si>
+    <t>GDP_raw_df</t>
+  </si>
+  <si>
+    <t>dataframe with the GDP information of countries of the world taken from the year 2019</t>
+  </si>
+  <si>
+    <t>income_url</t>
+  </si>
+  <si>
+    <t>my_params_2</t>
+  </si>
+  <si>
+    <t>url to communicate with the API from Worlbank with specific parameters to retrieve data on GDP of the countries</t>
+  </si>
+  <si>
+    <t>url to communicate with the API from Worlbank with specific parameters to retrieve data on income level of the countries</t>
+  </si>
+  <si>
+    <t>dictionary with paramters used for the API communication to get the GDP</t>
+  </si>
+  <si>
+    <t>dictionary with paramters used for the API communication to get the income level</t>
+  </si>
+  <si>
+    <t>r_income</t>
+  </si>
+  <si>
+    <t>r_gdp</t>
+  </si>
+  <si>
+    <t>requests.models.Response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">response object form the API on GDP data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">response object form the API on income level data </t>
+  </si>
+  <si>
+    <t>income_raw_df</t>
+  </si>
+  <si>
+    <t>dataframe with the Income level information of countries of the world taken from the current year</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>temporal dataframe from 'Confirmed', 'Deaths', 'Recovered' covid cases  grouped by country and date</t>
+  </si>
+  <si>
+    <t>mask</t>
+  </si>
+  <si>
+    <t>shifted by 1 dataframe from temp dataframe</t>
+  </si>
+  <si>
+    <t>cols</t>
+  </si>
+  <si>
+    <t>character list with the manes of the columns variables for calculating the new covid cases</t>
+  </si>
+  <si>
+    <t>my_final_df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataframe with time series of "clean" information on covid cases, stringency index and socioeconomicl data </t>
+  </si>
+  <si>
+    <t>covid/stringency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +367,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,23 +685,661 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD597728-7A71-FC46-BB6F-414CB7B6D2F7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="342" zoomScaleNormal="342" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="229" zoomScaleNormal="229" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>